<commit_message>
Changed Wenglor height relative uncertainty values
Decreased Wenglor relative height uncertainty from +/- 1 cm to +/- 1
mm.  Original value was too large.  The relative height uncertainty is
related to the positioning within the Wenglor array, which was
determined to high precision in the lab prior to deployment of the
array.  More of the height uncertainty (which is captured from the
distance sensor) is due to the position of the array relative to the
ground.
</commit_message>
<xml_diff>
--- a/Metadata/InstrumentMetadata_Oceano.xlsx
+++ b/Metadata/InstrumentMetadata_Oceano.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36440" yWindow="2100" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="33900" yWindow="1380" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,8 +375,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1519">
+  <cellStyleXfs count="1521">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1913,7 +1915,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1519">
+  <cellStyles count="1521">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2673,6 +2675,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1514" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1516" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1520" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3432,6 +3435,7 @@
     <cellStyle name="Hyperlink" xfId="1513" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1515" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1519" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3764,9 +3768,9 @@
   <dimension ref="A1:O648"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A642" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="M650" sqref="M650"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12975,7 +12979,7 @@
         <v>36</v>
       </c>
       <c r="G196" s="4">
-        <f t="shared" ref="G196:H217" si="1">0.64</f>
+        <f t="shared" ref="G196:G217" si="1">0.64</f>
         <v>0.64</v>
       </c>
       <c r="H196" s="4">
@@ -18520,7 +18524,7 @@
         <v>41</v>
       </c>
       <c r="G313" s="4">
-        <f t="shared" ref="G313:H334" si="3">8.95</f>
+        <f t="shared" ref="G313:G334" si="3">8.95</f>
         <v>8.9499999999999993</v>
       </c>
       <c r="H313" s="4">
@@ -27641,7 +27645,7 @@
         <v>-0.17</v>
       </c>
       <c r="I506" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J506" s="4" t="s">
         <v>9</v>
@@ -27688,7 +27692,7 @@
         <v>-0.17</v>
       </c>
       <c r="I507" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J507" s="4" t="s">
         <v>9</v>
@@ -27735,7 +27739,7 @@
         <v>-0.17</v>
       </c>
       <c r="I508" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J508" s="4" t="s">
         <v>9</v>
@@ -27782,7 +27786,7 @@
         <v>-0.17</v>
       </c>
       <c r="I509" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J509" s="4" t="s">
         <v>9</v>
@@ -27829,7 +27833,7 @@
         <v>-0.17</v>
       </c>
       <c r="I510" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J510" s="4" t="s">
         <v>9</v>
@@ -27876,7 +27880,7 @@
         <v>-0.17</v>
       </c>
       <c r="I511" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J511" s="4" t="s">
         <v>9</v>
@@ -27923,7 +27927,7 @@
         <v>-0.17</v>
       </c>
       <c r="I512" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J512" s="4" t="s">
         <v>9</v>
@@ -27970,7 +27974,7 @@
         <v>-0.17</v>
       </c>
       <c r="I513" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J513" s="4" t="s">
         <v>9</v>
@@ -28017,7 +28021,7 @@
         <v>-0.17</v>
       </c>
       <c r="I514" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J514" s="4" t="s">
         <v>9</v>
@@ -28064,7 +28068,7 @@
         <v>-0.17</v>
       </c>
       <c r="I515" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J515" s="4" t="s">
         <v>9</v>
@@ -28111,7 +28115,7 @@
         <v>-0.17</v>
       </c>
       <c r="I516" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J516" s="4" t="s">
         <v>9</v>
@@ -28158,7 +28162,7 @@
         <v>-0.17</v>
       </c>
       <c r="I517" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J517" s="4" t="s">
         <v>9</v>
@@ -28205,7 +28209,7 @@
         <v>-0.17</v>
       </c>
       <c r="I518" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J518" s="4" t="s">
         <v>9</v>
@@ -28252,7 +28256,7 @@
         <v>-0.17</v>
       </c>
       <c r="I519" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J519" s="4" t="s">
         <v>9</v>
@@ -28299,7 +28303,7 @@
         <v>-0.17</v>
       </c>
       <c r="I520" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J520" s="4" t="s">
         <v>9</v>
@@ -28346,7 +28350,7 @@
         <v>-0.17</v>
       </c>
       <c r="I521" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J521" s="4" t="s">
         <v>9</v>
@@ -28393,7 +28397,7 @@
         <v>-0.17</v>
       </c>
       <c r="I522" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J522" s="4" t="s">
         <v>9</v>
@@ -28440,7 +28444,7 @@
         <v>-0.17</v>
       </c>
       <c r="I523" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J523" s="4" t="s">
         <v>9</v>
@@ -28487,7 +28491,7 @@
         <v>-0.17</v>
       </c>
       <c r="I524" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J524" s="4" t="s">
         <v>9</v>
@@ -28534,7 +28538,7 @@
         <v>-0.17</v>
       </c>
       <c r="I525" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J525" s="4" t="s">
         <v>9</v>
@@ -28581,7 +28585,7 @@
         <v>-0.16</v>
       </c>
       <c r="I526" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J526" s="4" t="s">
         <v>9</v>
@@ -28628,7 +28632,7 @@
         <v>-0.16</v>
       </c>
       <c r="I527" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J527" s="4" t="s">
         <v>9</v>
@@ -28675,7 +28679,7 @@
         <v>-0.16</v>
       </c>
       <c r="I528" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J528" s="4" t="s">
         <v>9</v>
@@ -28722,7 +28726,7 @@
         <v>-0.16</v>
       </c>
       <c r="I529" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J529" s="4" t="s">
         <v>9</v>
@@ -28769,7 +28773,7 @@
         <v>-0.16</v>
       </c>
       <c r="I530" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J530" s="4" t="s">
         <v>9</v>
@@ -28816,7 +28820,7 @@
         <v>-0.16</v>
       </c>
       <c r="I531" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J531" s="4" t="s">
         <v>9</v>
@@ -28863,7 +28867,7 @@
         <v>-0.16</v>
       </c>
       <c r="I532" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J532" s="4" t="s">
         <v>9</v>
@@ -28910,7 +28914,7 @@
         <v>-0.16</v>
       </c>
       <c r="I533" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J533" s="4" t="s">
         <v>9</v>
@@ -28957,7 +28961,7 @@
         <v>-0.16</v>
       </c>
       <c r="I534" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J534" s="4" t="s">
         <v>9</v>
@@ -29004,7 +29008,7 @@
         <v>-0.16</v>
       </c>
       <c r="I535" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J535" s="4" t="s">
         <v>9</v>
@@ -29051,7 +29055,7 @@
         <v>-0.16</v>
       </c>
       <c r="I536" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J536" s="4" t="s">
         <v>9</v>
@@ -29098,7 +29102,7 @@
         <v>-0.16</v>
       </c>
       <c r="I537" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J537" s="4" t="s">
         <v>9</v>
@@ -29145,7 +29149,7 @@
         <v>-0.16</v>
       </c>
       <c r="I538" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J538" s="4" t="s">
         <v>9</v>
@@ -29192,7 +29196,7 @@
         <v>-0.16</v>
       </c>
       <c r="I539" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J539" s="4" t="s">
         <v>9</v>
@@ -29239,7 +29243,7 @@
         <v>-0.16</v>
       </c>
       <c r="I540" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J540" s="4" t="s">
         <v>9</v>
@@ -29286,7 +29290,7 @@
         <v>-0.16</v>
       </c>
       <c r="I541" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J541" s="4" t="s">
         <v>9</v>
@@ -29333,7 +29337,7 @@
         <v>-0.16</v>
       </c>
       <c r="I542" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J542" s="4" t="s">
         <v>9</v>
@@ -29380,7 +29384,7 @@
         <v>-0.16</v>
       </c>
       <c r="I543" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J543" s="4" t="s">
         <v>9</v>
@@ -29427,7 +29431,7 @@
         <v>-0.16</v>
       </c>
       <c r="I544" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J544" s="4" t="s">
         <v>9</v>
@@ -29474,7 +29478,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I545" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J545" s="4" t="s">
         <v>9</v>
@@ -29521,7 +29525,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I546" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J546" s="4" t="s">
         <v>9</v>
@@ -29568,7 +29572,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I547" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J547" s="4" t="s">
         <v>9</v>
@@ -29615,7 +29619,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I548" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J548" s="4" t="s">
         <v>9</v>
@@ -29662,7 +29666,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I549" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J549" s="4" t="s">
         <v>9</v>
@@ -29709,7 +29713,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I550" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J550" s="4" t="s">
         <v>9</v>
@@ -29756,7 +29760,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I551" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J551" s="4" t="s">
         <v>9</v>
@@ -29803,7 +29807,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I552" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J552" s="4" t="s">
         <v>9</v>
@@ -29850,7 +29854,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I553" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J553" s="4" t="s">
         <v>9</v>
@@ -29897,7 +29901,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I554" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J554" s="4" t="s">
         <v>9</v>
@@ -29944,7 +29948,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I555" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J555" s="4" t="s">
         <v>9</v>
@@ -29991,7 +29995,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I556" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J556" s="4" t="s">
         <v>9</v>
@@ -30038,7 +30042,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I557" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J557" s="4" t="s">
         <v>9</v>
@@ -30085,7 +30089,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I558" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J558" s="4" t="s">
         <v>9</v>
@@ -30132,7 +30136,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I559" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J559" s="4" t="s">
         <v>9</v>
@@ -30179,7 +30183,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I560" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J560" s="4" t="s">
         <v>9</v>
@@ -30226,7 +30230,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I561" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J561" s="4" t="s">
         <v>9</v>
@@ -30273,7 +30277,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I562" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J562" s="4" t="s">
         <v>9</v>
@@ -30320,7 +30324,7 @@
         <v>-0.14300000000000002</v>
       </c>
       <c r="I563" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J563" s="4" t="s">
         <v>9</v>
@@ -30367,7 +30371,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I564" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J564" s="4" t="s">
         <v>9</v>
@@ -30414,7 +30418,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I565" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J565" s="4" t="s">
         <v>9</v>
@@ -30461,7 +30465,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I566" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J566" s="4" t="s">
         <v>9</v>
@@ -30508,7 +30512,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I567" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J567" s="4" t="s">
         <v>9</v>
@@ -30555,7 +30559,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I568" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J568" s="4" t="s">
         <v>9</v>
@@ -30602,7 +30606,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I569" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J569" s="4" t="s">
         <v>9</v>
@@ -30649,7 +30653,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I570" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J570" s="4" t="s">
         <v>9</v>
@@ -30696,7 +30700,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I571" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J571" s="4" t="s">
         <v>9</v>
@@ -30743,7 +30747,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I572" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J572" s="4" t="s">
         <v>9</v>
@@ -30790,7 +30794,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I573" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J573" s="4" t="s">
         <v>9</v>
@@ -30837,7 +30841,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I574" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J574" s="4" t="s">
         <v>9</v>
@@ -30884,7 +30888,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I575" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J575" s="4" t="s">
         <v>9</v>
@@ -30931,7 +30935,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I576" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J576" s="4" t="s">
         <v>9</v>
@@ -30978,7 +30982,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I577" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J577" s="4" t="s">
         <v>9</v>
@@ -31025,7 +31029,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I578" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J578" s="4" t="s">
         <v>9</v>
@@ -31072,7 +31076,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I579" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J579" s="4" t="s">
         <v>9</v>
@@ -31119,7 +31123,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I580" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J580" s="4" t="s">
         <v>9</v>
@@ -31166,7 +31170,7 @@
         <v>-0.11800000000000001</v>
       </c>
       <c r="I581" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J581" s="4" t="s">
         <v>9</v>
@@ -31213,7 +31217,7 @@
         <v>-0.09</v>
       </c>
       <c r="I582" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J582" s="4" t="s">
         <v>9</v>
@@ -31260,7 +31264,7 @@
         <v>-0.09</v>
       </c>
       <c r="I583" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J583" s="4" t="s">
         <v>9</v>
@@ -31307,7 +31311,7 @@
         <v>-0.09</v>
       </c>
       <c r="I584" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J584" s="4" t="s">
         <v>9</v>
@@ -31354,7 +31358,7 @@
         <v>-0.09</v>
       </c>
       <c r="I585" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J585" s="4" t="s">
         <v>9</v>
@@ -31401,7 +31405,7 @@
         <v>-0.09</v>
       </c>
       <c r="I586" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J586" s="4" t="s">
         <v>9</v>
@@ -31448,7 +31452,7 @@
         <v>-0.09</v>
       </c>
       <c r="I587" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J587" s="4" t="s">
         <v>9</v>
@@ -31495,7 +31499,7 @@
         <v>-0.09</v>
       </c>
       <c r="I588" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J588" s="4" t="s">
         <v>9</v>
@@ -31542,7 +31546,7 @@
         <v>-0.09</v>
       </c>
       <c r="I589" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J589" s="4" t="s">
         <v>9</v>
@@ -31589,7 +31593,7 @@
         <v>-0.09</v>
       </c>
       <c r="I590" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J590" s="4" t="s">
         <v>9</v>
@@ -31636,7 +31640,7 @@
         <v>-0.09</v>
       </c>
       <c r="I591" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J591" s="4" t="s">
         <v>9</v>
@@ -31683,7 +31687,7 @@
         <v>-0.09</v>
       </c>
       <c r="I592" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J592" s="4" t="s">
         <v>9</v>
@@ -31730,7 +31734,7 @@
         <v>-0.09</v>
       </c>
       <c r="I593" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J593" s="4" t="s">
         <v>9</v>
@@ -31777,7 +31781,7 @@
         <v>-0.09</v>
       </c>
       <c r="I594" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J594" s="4" t="s">
         <v>9</v>
@@ -31824,7 +31828,7 @@
         <v>-0.05</v>
       </c>
       <c r="I595" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J595" s="4" t="s">
         <v>9</v>
@@ -31871,7 +31875,7 @@
         <v>-0.05</v>
       </c>
       <c r="I596" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J596" s="4" t="s">
         <v>9</v>
@@ -31918,7 +31922,7 @@
         <v>-0.05</v>
       </c>
       <c r="I597" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J597" s="4" t="s">
         <v>9</v>
@@ -31965,7 +31969,7 @@
         <v>-0.05</v>
       </c>
       <c r="I598" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J598" s="4" t="s">
         <v>9</v>
@@ -32012,7 +32016,7 @@
         <v>-0.05</v>
       </c>
       <c r="I599" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J599" s="4" t="s">
         <v>9</v>
@@ -32059,7 +32063,7 @@
         <v>-0.05</v>
       </c>
       <c r="I600" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J600" s="4" t="s">
         <v>9</v>
@@ -32106,7 +32110,7 @@
         <v>-0.05</v>
       </c>
       <c r="I601" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J601" s="4" t="s">
         <v>9</v>
@@ -32153,7 +32157,7 @@
         <v>-0.05</v>
       </c>
       <c r="I602" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J602" s="4" t="s">
         <v>9</v>
@@ -32200,7 +32204,7 @@
         <v>-0.05</v>
       </c>
       <c r="I603" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J603" s="4" t="s">
         <v>9</v>
@@ -32247,7 +32251,7 @@
         <v>-0.05</v>
       </c>
       <c r="I604" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J604" s="4" t="s">
         <v>9</v>
@@ -32294,7 +32298,7 @@
         <v>-0.05</v>
       </c>
       <c r="I605" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J605" s="4" t="s">
         <v>9</v>
@@ -32341,7 +32345,7 @@
         <v>-0.05</v>
       </c>
       <c r="I606" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J606" s="4" t="s">
         <v>9</v>
@@ -32388,7 +32392,7 @@
         <v>-0.05</v>
       </c>
       <c r="I607" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J607" s="4" t="s">
         <v>9</v>
@@ -32435,7 +32439,7 @@
         <v>0.01</v>
       </c>
       <c r="I608" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J608" s="4" t="s">
         <v>9</v>
@@ -32482,7 +32486,7 @@
         <v>0.01</v>
       </c>
       <c r="I609" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J609" s="4" t="s">
         <v>9</v>
@@ -32529,7 +32533,7 @@
         <v>0.01</v>
       </c>
       <c r="I610" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J610" s="4" t="s">
         <v>9</v>
@@ -32576,7 +32580,7 @@
         <v>0.01</v>
       </c>
       <c r="I611" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J611" s="4" t="s">
         <v>9</v>
@@ -32623,7 +32627,7 @@
         <v>0.01</v>
       </c>
       <c r="I612" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J612" s="4" t="s">
         <v>9</v>
@@ -32670,7 +32674,7 @@
         <v>0.01</v>
       </c>
       <c r="I613" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J613" s="4" t="s">
         <v>9</v>
@@ -32717,7 +32721,7 @@
         <v>0.01</v>
       </c>
       <c r="I614" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J614" s="4" t="s">
         <v>9</v>
@@ -32764,7 +32768,7 @@
         <v>0.01</v>
       </c>
       <c r="I615" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J615" s="4" t="s">
         <v>9</v>
@@ -32811,7 +32815,7 @@
         <v>0.01</v>
       </c>
       <c r="I616" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J616" s="4" t="s">
         <v>9</v>
@@ -32858,7 +32862,7 @@
         <v>0.01</v>
       </c>
       <c r="I617" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J617" s="4" t="s">
         <v>9</v>
@@ -32905,7 +32909,7 @@
         <v>0.01</v>
       </c>
       <c r="I618" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J618" s="4" t="s">
         <v>9</v>
@@ -32952,7 +32956,7 @@
         <v>0.01</v>
       </c>
       <c r="I619" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J619" s="4" t="s">
         <v>9</v>
@@ -32999,7 +33003,7 @@
         <v>0.01</v>
       </c>
       <c r="I620" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J620" s="4" t="s">
         <v>9</v>
@@ -33046,7 +33050,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I621" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J621" s="4" t="s">
         <v>9</v>
@@ -33093,7 +33097,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I622" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J622" s="4" t="s">
         <v>9</v>
@@ -33140,7 +33144,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I623" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J623" s="4" t="s">
         <v>9</v>
@@ -33187,7 +33191,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I624" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J624" s="4" t="s">
         <v>9</v>
@@ -33234,7 +33238,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I625" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J625" s="4" t="s">
         <v>9</v>
@@ -33281,7 +33285,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I626" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J626" s="4" t="s">
         <v>9</v>
@@ -33328,7 +33332,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I627" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J627" s="4" t="s">
         <v>9</v>
@@ -33375,7 +33379,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I628" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J628" s="4" t="s">
         <v>9</v>
@@ -33422,7 +33426,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I629" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J629" s="4" t="s">
         <v>9</v>
@@ -33469,7 +33473,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I630" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J630" s="4" t="s">
         <v>9</v>
@@ -33516,7 +33520,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I631" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J631" s="4" t="s">
         <v>9</v>
@@ -33563,7 +33567,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I632" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J632" s="4" t="s">
         <v>9</v>
@@ -33610,7 +33614,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I633" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J633" s="4" t="s">
         <v>9</v>
@@ -33657,7 +33661,7 @@
         <v>9.9000000000000019E-2</v>
       </c>
       <c r="I634" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J634" s="4" t="s">
         <v>9</v>
@@ -33704,7 +33708,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I635" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J635" s="4" t="s">
         <v>9</v>
@@ -33751,7 +33755,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I636" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J636" s="4" t="s">
         <v>9</v>
@@ -33798,7 +33802,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I637" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J637" s="4" t="s">
         <v>9</v>
@@ -33845,7 +33849,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I638" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J638" s="4" t="s">
         <v>9</v>
@@ -33892,7 +33896,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I639" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J639" s="4" t="s">
         <v>9</v>
@@ -33939,7 +33943,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I640" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J640" s="4" t="s">
         <v>9</v>
@@ -33986,7 +33990,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I641" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J641" s="4" t="s">
         <v>9</v>
@@ -34033,7 +34037,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I642" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J642" s="4" t="s">
         <v>9</v>
@@ -34080,7 +34084,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I643" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J643" s="4" t="s">
         <v>9</v>
@@ -34127,7 +34131,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I644" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J644" s="4" t="s">
         <v>9</v>
@@ -34174,7 +34178,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I645" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J645" s="4" t="s">
         <v>9</v>
@@ -34221,7 +34225,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I646" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J646" s="4" t="s">
         <v>9</v>
@@ -34268,7 +34272,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I647" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J647" s="4" t="s">
         <v>9</v>
@@ -34315,7 +34319,7 @@
         <v>0.22699999999999998</v>
       </c>
       <c r="I648" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J648" s="4" t="s">
         <v>9</v>

</xml_diff>